<commit_message>
transforms: excel to frontend needs
</commit_message>
<xml_diff>
--- a/server/data/final/miscellaneousData.xlsx
+++ b/server/data/final/miscellaneousData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="15255" windowHeight="4635"/>
+    <workbookView xWindow="480" yWindow="345" windowWidth="19815" windowHeight="7665"/>
   </bookViews>
   <sheets>
     <sheet name="misc" sheetId="1" r:id="rId1"/>
@@ -1872,16 +1872,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I356"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C356" sqref="C356"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">

</xml_diff>